<commit_message>
Updated boms for Word compatibility, updating user guide
</commit_message>
<xml_diff>
--- a/hardware/dispenser/bom/precise_dispenser_bom.xlsx
+++ b/hardware/dispenser/bom/precise_dispenser_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub Repos\canine_precise_dispenser\hardware\dispenser\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFCB6D5-FDE8-4215-8141-4D96282FBD3D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C679A6-07C2-4906-9EAD-8F491D791D38}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Bill of Materials - Precise Dispenser</t>
   </si>
@@ -90,61 +90,13 @@
     <t>Cable Ties</t>
   </si>
   <si>
-    <t>https://www.amazon.com/gp/product/B08F77YVYB/ref=ppx_yo_dt_b_asin_title_o00_s00?ie=UTF8&amp;psc=1</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/gp/product/B06XP16Q4W/ref=ppx_yo_dt_b_asin_title_o01_s00?ie=UTF8&amp;th=1</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/gp/product/B083SGJ7BD/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1</t>
-  </si>
-  <si>
-    <t>https://www.adafruit.com/product/2167</t>
-  </si>
-  <si>
-    <t>https://www.sparkfun.com/products/15448</t>
-  </si>
-  <si>
-    <t>https://www.sparkfun.com/products/15447</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/10-02879/839-1449-ND/8635386?itemSeq=352933944</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/4261/1528-4261-ND/10287031?itemSeq=352933946</t>
-  </si>
-  <si>
-    <t>https://www.digikey.com/en/products/detail/4054/1528-2888-ND/9997693?itemSeq=352933947</t>
-  </si>
-  <si>
     <t>Stepper Motor Power Supply</t>
   </si>
   <si>
-    <t>https://www.digikey.com/en/products/detail/tensility-international-corp/16-00143/10324430</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/OVERTURE-Filament-Consumables-Dimensional-Accuracy/dp/B07PGY2JP1/ref=sr_1_9?crid=SP2VJ9AX94HN&amp;dchild=1&amp;keywords=1kg+pla+filament+1.75mm&amp;qid=1612737824&amp;sprefix=1kg+pla+%2Caps%2C223&amp;sr=8-9</t>
-  </si>
-  <si>
     <t>Micro SD Card</t>
   </si>
   <si>
-    <t>https://www.amazon.com/Micro-Center-Class-Memory-Adapter/dp/B07K835MNR/ref=sr_1_36?dchild=1&amp;keywords=16gb+sd+card&amp;qid=1612732635&amp;sr=8-36</t>
-  </si>
-  <si>
     <t>USB C Cable</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/JXMOX-Charger-Charging-Compatible-2018-Grey/dp/B07TVMBZ75/ref=sr_1_3?dchild=1&amp;keywords=usb+c+to+usb+c+cable+short&amp;qid=1612732867&amp;sr=8-3</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/GANA-Adapter-Female-Action-Supported/dp/B07K21HSQX/ref=sr_1_3?dchild=1&amp;keywords=micro+hdmi+to+hdmi+female&amp;qid=1612730938&amp;sr=8-3</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/gp/product/B087BWKJZP/ref=ox_sc_act_title_1?smid=A2TMK1RHV496EY&amp;th=1</t>
-  </si>
-  <si>
-    <t>https://www.amazon.com/gp/product/B083HNZWK6/ref=ox_sc_act_title_2?smid=A2PYYAAPQIARBH&amp;psc=1</t>
   </si>
 </sst>
 </file>
@@ -154,7 +106,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -169,6 +121,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -178,7 +144,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -186,20 +152,77 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="fill"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -480,16 +503,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -497,248 +521,283 @@
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
+    <row r="2" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="4">
         <v>22.99</v>
       </c>
-      <c r="D3" t="s">
-        <v>29</v>
+      <c r="D3" s="9" t="str">
+        <f>HYPERLINK("https://www.amazon.com/OVERTURE-Filament-Consumables-Dimensional-Accuracy/dp/B07PGY2JP1/ref=sr_1_9?crid=SP2VJ9AX94HN&amp;dchild=1&amp;keywords=1kg+pla+filament+1.75mm&amp;qid=1612737824&amp;sprefix=1kg+pla+%2Caps%2C223&amp;sr=8-9","Filament")</f>
+        <v>Filament</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="A4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="5">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6">
         <v>55</v>
       </c>
-      <c r="D4" t="s">
-        <v>23</v>
+      <c r="D4" s="10" t="str">
+        <f>HYPERLINK("https://www.sparkfun.com/products/15447","Raspberry Pi")</f>
+        <v>Raspberry Pi</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="A5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2">
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="6">
         <v>7.95</v>
       </c>
-      <c r="D5" t="s">
-        <v>26</v>
+      <c r="D5" s="10" t="str">
+        <f>HYPERLINK("https://www.digikey.com/en/products/detail/4054/1528-2888-ND/9997693?itemSeq=352933947","HDMI")</f>
+        <v>HDMI</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="B6" s="5">
+        <v>1</v>
+      </c>
+      <c r="C6" s="6">
         <v>7.5</v>
       </c>
-      <c r="D6" t="s">
-        <v>25</v>
+      <c r="D6" s="10" t="str">
+        <f>HYPERLINK("https://www.digikey.com/en/products/detail/4261/1528-4261-ND/10287031?itemSeq=352933946","USB C")</f>
+        <v>USB C</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+      <c r="A7" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2">
+      <c r="B7" s="5">
+        <v>1</v>
+      </c>
+      <c r="C7" s="6">
         <v>5.17</v>
       </c>
-      <c r="D7" t="s">
-        <v>24</v>
+      <c r="D7" s="10" t="str">
+        <f>HYPERLINK("https://www.digikey.com/en/products/detail/10-02879/839-1449-ND/8635386?itemSeq=352933944","Barrel Jack")</f>
+        <v>Barrel Jack</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+      <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2">
+      <c r="B8" s="5">
+        <v>1</v>
+      </c>
+      <c r="C8" s="6">
         <v>8.69</v>
       </c>
-      <c r="D8" t="s">
-        <v>34</v>
+      <c r="D8" s="10" t="str">
+        <f>HYPERLINK("https://www.amazon.com/GANA-Adapter-Female-Action-Supported/dp/B07K21HSQX/ref=sr_1_3?dchild=1&amp;keywords=micro+hdmi+to+hdmi+female&amp;qid=1612730938&amp;sr=8-3","Micro HDMI")</f>
+        <v>Micro HDMI</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>27</v>
-      </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" s="2">
+      <c r="A9" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="5">
+        <v>1</v>
+      </c>
+      <c r="C9" s="6">
         <v>11.61</v>
       </c>
-      <c r="D9" t="s">
-        <v>28</v>
+      <c r="D9" s="10" t="str">
+        <f>HYPERLINK("https://www.digikey.com/en/products/detail/tensility-international-corp/16-00143/10324430", "12V Power")</f>
+        <v>12V Power</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="A10" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" s="2">
+      <c r="B10" s="5">
+        <v>1</v>
+      </c>
+      <c r="C10" s="6">
         <v>8.99</v>
       </c>
-      <c r="D10" t="s">
-        <v>35</v>
+      <c r="D10" s="10" t="str">
+        <f>HYPERLINK("https://www.amazon.com/gp/product/B087BWKJZP/ref=ox_sc_act_title_1?smid=A2TMK1RHV496EY&amp;th=1","Motor")</f>
+        <v>Motor</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" s="2">
+      <c r="B11" s="5">
+        <v>1</v>
+      </c>
+      <c r="C11" s="6">
         <v>8</v>
       </c>
-      <c r="D11" t="s">
-        <v>22</v>
+      <c r="D11" s="10" t="str">
+        <f>HYPERLINK("https://www.sparkfun.com/products/15448","Pi Power")</f>
+        <v>Pi Power</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="A12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" s="2">
+      <c r="B12" s="5">
+        <v>1</v>
+      </c>
+      <c r="C12" s="6">
         <v>9.9499999999999993</v>
       </c>
-      <c r="D12" t="s">
-        <v>36</v>
+      <c r="D12" s="10" t="str">
+        <f>HYPERLINK("https://www.amazon.com/gp/product/B083HNZWK6/ref=ox_sc_act_title_2?smid=A2PYYAAPQIARBH&amp;psc=1","8 in Cover")</f>
+        <v>8 in Cover</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="A13" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="2">
+      <c r="B13" s="5">
+        <v>1</v>
+      </c>
+      <c r="C13" s="6">
         <v>1.95</v>
       </c>
-      <c r="D13" t="s">
-        <v>21</v>
+      <c r="D13" s="10" t="str">
+        <f>HYPERLINK("https://www.adafruit.com/product/2167","3mm IR")</f>
+        <v>3mm IR</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
+      <c r="A14" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B14">
-        <v>1</v>
-      </c>
-      <c r="C14" s="2">
+      <c r="B14" s="5">
+        <v>1</v>
+      </c>
+      <c r="C14" s="6">
         <v>26.99</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="10" t="str">
+        <f>HYPERLINK("https://www.amazon.com/gp/product/B083SGJ7BD/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1","M3 Pack")</f>
+        <v>M3 Pack</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" s="5">
+        <v>1</v>
+      </c>
+      <c r="C15" s="6">
+        <v>14.99</v>
+      </c>
+      <c r="D15" s="10" t="str">
+        <f>HYPERLINK("https://www.amazon.com/gp/product/B06XP16Q4W/ref=ppx_yo_dt_b_asin_title_o01_s00?ie=UTF8&amp;th=1","Hex Set")</f>
+        <v>Hex Set</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" s="6">
+        <v>9.69</v>
+      </c>
+      <c r="D16" s="10" t="str">
+        <f>HYPERLINK("https://www.amazon.com/gp/product/B08F77YVYB/ref=ppx_yo_dt_b_asin_title_o00_s00?ie=UTF8&amp;psc=1", "Zip Ties and Mounts")</f>
+        <v>Zip Ties and Mounts</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B17" s="5">
+        <v>1</v>
+      </c>
+      <c r="C17" s="6">
+        <v>9.49</v>
+      </c>
+      <c r="D17" s="10" t="str">
+        <f>HYPERLINK("https://www.amazon.com/Micro-Center-Class-Memory-Adapter/dp/B07K835MNR/ref=sr_1_36?dchild=1&amp;keywords=16gb+sd+card&amp;qid=1612732635&amp;sr=8-36","SD Card Pack")</f>
+        <v>SD Card Pack</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15">
-        <v>1</v>
-      </c>
-      <c r="C15" s="2">
-        <v>14.99</v>
-      </c>
-      <c r="D15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" s="2">
-        <v>9.69</v>
-      </c>
-      <c r="D16" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>30</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2">
-        <v>9.49</v>
-      </c>
-      <c r="D17" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>32</v>
-      </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" s="2">
+      <c r="B18" s="7">
+        <v>1</v>
+      </c>
+      <c r="C18" s="8">
         <v>6.99</v>
       </c>
-      <c r="D18" t="s">
-        <v>33</v>
+      <c r="D18" s="11" t="str">
+        <f>HYPERLINK("https://www.amazon.com/JXMOX-Charger-Charging-Compatible-2018-Grey/dp/B07TVMBZ75/ref=sr_1_3?dchild=1&amp;keywords=usb+c+to+usb+c+cable+short&amp;qid=1612732867&amp;sr=8-3","USB C Cables")</f>
+        <v>USB C Cables</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="D3" r:id="rId1" display="https://www.amazon.com/OVERTURE-Filament-Consumables-Dimensional-Accuracy/dp/B07PGY2JP1/ref=sr_1_9?crid=SP2VJ9AX94HN&amp;dchild=1&amp;keywords=1kg+pla+filament+1.75mm&amp;qid=1612737824&amp;sprefix=1kg+pla+%2Caps%2C223&amp;sr=8-9" xr:uid="{E662DE8F-55B9-4DE4-9151-29E4BE09A5B0}"/>
+    <hyperlink ref="D4" r:id="rId2" display="https://www.sparkfun.com/products/15447" xr:uid="{55A3649E-3EA4-403A-918D-36FE8F8441A3}"/>
+    <hyperlink ref="D5" r:id="rId3" display="https://www.digikey.com/en/products/detail/4054/1528-2888-ND/9997693?itemSeq=352933947" xr:uid="{90C56143-1A0C-4410-B500-68740161FC6B}"/>
+    <hyperlink ref="D6" r:id="rId4" display="https://www.digikey.com/en/products/detail/4261/1528-4261-ND/10287031?itemSeq=352933946" xr:uid="{5C372F36-28B8-43E7-BED3-F751590B6BF5}"/>
+    <hyperlink ref="D7" r:id="rId5" display="https://www.digikey.com/en/products/detail/10-02879/839-1449-ND/8635386?itemSeq=352933944" xr:uid="{8576396F-AE3A-4B20-8024-DA6E9AAD6342}"/>
+    <hyperlink ref="D8" r:id="rId6" display="https://www.amazon.com/GANA-Adapter-Female-Action-Supported/dp/B07K21HSQX/ref=sr_1_3?dchild=1&amp;keywords=micro+hdmi+to+hdmi+female&amp;qid=1612730938&amp;sr=8-3" xr:uid="{B641A4D8-171A-4FC8-A197-21BF8B4F2744}"/>
+    <hyperlink ref="D9" r:id="rId7" display="https://www.digikey.com/en/products/detail/tensility-international-corp/16-00143/10324430" xr:uid="{5A97FF7F-C50D-406A-A38D-74E57DCAC5FB}"/>
+    <hyperlink ref="D10" r:id="rId8" display="https://www.amazon.com/gp/product/B087BWKJZP/ref=ox_sc_act_title_1?smid=A2TMK1RHV496EY&amp;th=1" xr:uid="{21D61FE2-4A9D-46E0-9E96-C42C6DA1CE4F}"/>
+    <hyperlink ref="D12" r:id="rId9" display="https://www.amazon.com/gp/product/B083HNZWK6/ref=ox_sc_act_title_2?smid=A2PYYAAPQIARBH&amp;psc=1" xr:uid="{B71808F8-FCFB-42D3-BF52-58D9E0580C1A}"/>
+    <hyperlink ref="D14" r:id="rId10" display="https://www.amazon.com/gp/product/B083SGJ7BD/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1" xr:uid="{DA66DF38-A09F-4211-8141-1818E8E255C7}"/>
+    <hyperlink ref="D15" r:id="rId11" display="https://www.amazon.com/gp/product/B06XP16Q4W/ref=ppx_yo_dt_b_asin_title_o01_s00?ie=UTF8&amp;th=1" xr:uid="{FF29243F-9608-467D-869E-7514D665C27E}"/>
+    <hyperlink ref="D16" r:id="rId12" display="https://www.amazon.com/gp/product/B08F77YVYB/ref=ppx_yo_dt_b_asin_title_o00_s00?ie=UTF8&amp;psc=1" xr:uid="{0751953C-478C-4815-94D1-AC08779238DF}"/>
+    <hyperlink ref="D17" r:id="rId13" display="https://www.amazon.com/Micro-Center-Class-Memory-Adapter/dp/B07K835MNR/ref=sr_1_36?dchild=1&amp;keywords=16gb+sd+card&amp;qid=1612732635&amp;sr=8-36" xr:uid="{0ED02E94-4D76-4658-8DE0-18A017F4CBA8}"/>
+    <hyperlink ref="D18" r:id="rId14" display="https://www.amazon.com/JXMOX-Charger-Charging-Compatible-2018-Grey/dp/B07TVMBZ75/ref=sr_1_3?dchild=1&amp;keywords=usb+c+to+usb+c+cable+short&amp;qid=1612732867&amp;sr=8-3" xr:uid="{A65511AB-084D-482E-ACC8-8AC38907AF9B}"/>
+    <hyperlink ref="D11" r:id="rId15" display="https://www.sparkfun.com/products/15448" xr:uid="{9716C4E0-BADF-4347-8019-72F83F0A0FEC}"/>
+    <hyperlink ref="D13" r:id="rId16" display="https://www.adafruit.com/product/2167" xr:uid="{F390DA11-248B-4D88-B312-4E370CAC65D6}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Sliced the last of the dispenser files
</commit_message>
<xml_diff>
--- a/hardware/dispenser/bom/precise_dispenser_bom.xlsx
+++ b/hardware/dispenser/bom/precise_dispenser_bom.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub Repos\canine_precise_dispenser\hardware\dispenser\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C679A6-07C2-4906-9EAD-8F491D791D38}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5F17ED5-9A02-415E-A751-B4416CC465A3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Bill of Materials - Precise Dispenser</t>
   </si>
@@ -82,9 +82,6 @@
   </si>
   <si>
     <t>M3 Screws</t>
-  </si>
-  <si>
-    <t>M3 Hex Wrench</t>
   </si>
   <si>
     <t>Cable Ties</t>
@@ -200,9 +197,6 @@
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1"/>
@@ -218,6 +212,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="fill"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -501,10 +498,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D18"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -514,264 +511,249 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="A2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
         <v>22.99</v>
       </c>
-      <c r="D3" s="9" t="str">
+      <c r="D3" s="8" t="str">
         <f>HYPERLINK("https://www.amazon.com/OVERTURE-Filament-Consumables-Dimensional-Accuracy/dp/B07PGY2JP1/ref=sr_1_9?crid=SP2VJ9AX94HN&amp;dchild=1&amp;keywords=1kg+pla+filament+1.75mm&amp;qid=1612737824&amp;sprefix=1kg+pla+%2Caps%2C223&amp;sr=8-9","Filament")</f>
         <v>Filament</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="5">
-        <v>1</v>
-      </c>
-      <c r="C4" s="6">
+      <c r="B4" s="4">
+        <v>1</v>
+      </c>
+      <c r="C4" s="5">
         <v>55</v>
       </c>
-      <c r="D4" s="10" t="str">
+      <c r="D4" s="9" t="str">
         <f>HYPERLINK("https://www.sparkfun.com/products/15447","Raspberry Pi")</f>
         <v>Raspberry Pi</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5">
-        <v>1</v>
-      </c>
-      <c r="C5" s="6">
+      <c r="B5" s="4">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
         <v>7.95</v>
       </c>
-      <c r="D5" s="10" t="str">
+      <c r="D5" s="9" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/4054/1528-2888-ND/9997693?itemSeq=352933947","HDMI")</f>
         <v>HDMI</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="5">
-        <v>1</v>
-      </c>
-      <c r="C6" s="6">
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="5">
         <v>7.5</v>
       </c>
-      <c r="D6" s="10" t="str">
+      <c r="D6" s="9" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/4261/1528-4261-ND/10287031?itemSeq=352933946","USB C")</f>
         <v>USB C</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="5">
-        <v>1</v>
-      </c>
-      <c r="C7" s="6">
+      <c r="B7" s="4">
+        <v>1</v>
+      </c>
+      <c r="C7" s="5">
         <v>5.17</v>
       </c>
-      <c r="D7" s="10" t="str">
+      <c r="D7" s="9" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/10-02879/839-1449-ND/8635386?itemSeq=352933944","Barrel Jack")</f>
         <v>Barrel Jack</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="5">
-        <v>1</v>
-      </c>
-      <c r="C8" s="6">
+      <c r="B8" s="4">
+        <v>1</v>
+      </c>
+      <c r="C8" s="5">
         <v>8.69</v>
       </c>
-      <c r="D8" s="10" t="str">
+      <c r="D8" s="9" t="str">
         <f>HYPERLINK("https://www.amazon.com/GANA-Adapter-Female-Action-Supported/dp/B07K21HSQX/ref=sr_1_3?dchild=1&amp;keywords=micro+hdmi+to+hdmi+female&amp;qid=1612730938&amp;sr=8-3","Micro HDMI")</f>
         <v>Micro HDMI</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="5">
-        <v>1</v>
-      </c>
-      <c r="C9" s="6">
+      <c r="A9" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1</v>
+      </c>
+      <c r="C9" s="5">
         <v>11.61</v>
       </c>
-      <c r="D9" s="10" t="str">
+      <c r="D9" s="9" t="str">
         <f>HYPERLINK("https://www.digikey.com/en/products/detail/tensility-international-corp/16-00143/10324430", "12V Power")</f>
         <v>12V Power</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="5">
-        <v>1</v>
-      </c>
-      <c r="C10" s="6">
+      <c r="B10" s="4">
+        <v>1</v>
+      </c>
+      <c r="C10" s="5">
         <v>8.99</v>
       </c>
-      <c r="D10" s="10" t="str">
+      <c r="D10" s="9" t="str">
         <f>HYPERLINK("https://www.amazon.com/gp/product/B087BWKJZP/ref=ox_sc_act_title_1?smid=A2TMK1RHV496EY&amp;th=1","Motor")</f>
         <v>Motor</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="5">
-        <v>1</v>
-      </c>
-      <c r="C11" s="6">
+      <c r="B11" s="4">
+        <v>1</v>
+      </c>
+      <c r="C11" s="5">
         <v>8</v>
       </c>
-      <c r="D11" s="10" t="str">
+      <c r="D11" s="9" t="str">
         <f>HYPERLINK("https://www.sparkfun.com/products/15448","Pi Power")</f>
         <v>Pi Power</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="5">
-        <v>1</v>
-      </c>
-      <c r="C12" s="6">
+      <c r="B12" s="4">
+        <v>1</v>
+      </c>
+      <c r="C12" s="5">
         <v>9.9499999999999993</v>
       </c>
-      <c r="D12" s="10" t="str">
+      <c r="D12" s="9" t="str">
         <f>HYPERLINK("https://www.amazon.com/gp/product/B083HNZWK6/ref=ox_sc_act_title_2?smid=A2PYYAAPQIARBH&amp;psc=1","8 in Cover")</f>
         <v>8 in Cover</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="5">
-        <v>1</v>
-      </c>
-      <c r="C13" s="6">
+      <c r="B13" s="4">
+        <v>1</v>
+      </c>
+      <c r="C13" s="5">
         <v>1.95</v>
       </c>
-      <c r="D13" s="10" t="str">
+      <c r="D13" s="9" t="str">
         <f>HYPERLINK("https://www.adafruit.com/product/2167","3mm IR")</f>
         <v>3mm IR</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="5">
-        <v>1</v>
-      </c>
-      <c r="C14" s="6">
+      <c r="B14" s="4">
+        <v>1</v>
+      </c>
+      <c r="C14" s="5">
         <v>26.99</v>
       </c>
-      <c r="D14" s="10" t="str">
+      <c r="D14" s="9" t="str">
         <f>HYPERLINK("https://www.amazon.com/gp/product/B083SGJ7BD/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1","M3 Pack")</f>
         <v>M3 Pack</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="5">
-        <v>1</v>
-      </c>
-      <c r="C15" s="6">
-        <v>14.99</v>
-      </c>
-      <c r="D15" s="10" t="str">
-        <f>HYPERLINK("https://www.amazon.com/gp/product/B06XP16Q4W/ref=ppx_yo_dt_b_asin_title_o01_s00?ie=UTF8&amp;th=1","Hex Set")</f>
-        <v>Hex Set</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="5">
-        <v>1</v>
-      </c>
-      <c r="C16" s="6">
+      <c r="B15" s="4">
+        <v>1</v>
+      </c>
+      <c r="C15" s="5">
         <v>9.69</v>
       </c>
-      <c r="D16" s="10" t="str">
+      <c r="D15" s="9" t="str">
         <f>HYPERLINK("https://www.amazon.com/gp/product/B08F77YVYB/ref=ppx_yo_dt_b_asin_title_o00_s00?ie=UTF8&amp;psc=1", "Zip Ties and Mounts")</f>
         <v>Zip Ties and Mounts</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1</v>
+      </c>
+      <c r="C16" s="5">
+        <v>6.49</v>
+      </c>
+      <c r="D16" s="9" t="str">
+        <f>HYPERLINK("https://www.amazon.com/Micro-Center-Class-Memory-Adapter/dp/B07YLYX4NL/ref=sr_1_36?dchild=1&amp;keywords=16gb%2Bsd%2Bcard&amp;qid=1612732635&amp;sr=8-36&amp;th=1","SD Card Pack")</f>
+        <v>SD Card Pack</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="5">
-        <v>1</v>
-      </c>
-      <c r="C17" s="6">
-        <v>9.49</v>
+      <c r="B17" s="6">
+        <v>1</v>
+      </c>
+      <c r="C17" s="7">
+        <v>6.99</v>
       </c>
       <c r="D17" s="10" t="str">
-        <f>HYPERLINK("https://www.amazon.com/Micro-Center-Class-Memory-Adapter/dp/B07K835MNR/ref=sr_1_36?dchild=1&amp;keywords=16gb+sd+card&amp;qid=1612732635&amp;sr=8-36","SD Card Pack")</f>
-        <v>SD Card Pack</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="7">
-        <v>1</v>
-      </c>
-      <c r="C18" s="8">
-        <v>6.99</v>
-      </c>
-      <c r="D18" s="11" t="str">
-        <f>HYPERLINK("https://www.amazon.com/JXMOX-Charger-Charging-Compatible-2018-Grey/dp/B07TVMBZ75/ref=sr_1_3?dchild=1&amp;keywords=usb+c+to+usb+c+cable+short&amp;qid=1612732867&amp;sr=8-3","USB C Cables")</f>
+        <f>HYPERLINK("https://www.amazon.com/Charging-Durable-Station-Compatible-Samsung/dp/B08LL1SVZD/ref=sr_1_128?dchild=1&amp;keywords=usb+c+cable&amp;qid=1618609001&amp;s=electronics&amp;sr=1-128","USB C Cables")</f>
         <v>USB C Cables</v>
       </c>
     </row>
@@ -790,14 +772,13 @@
     <hyperlink ref="D10" r:id="rId8" display="https://www.amazon.com/gp/product/B087BWKJZP/ref=ox_sc_act_title_1?smid=A2TMK1RHV496EY&amp;th=1" xr:uid="{21D61FE2-4A9D-46E0-9E96-C42C6DA1CE4F}"/>
     <hyperlink ref="D12" r:id="rId9" display="https://www.amazon.com/gp/product/B083HNZWK6/ref=ox_sc_act_title_2?smid=A2PYYAAPQIARBH&amp;psc=1" xr:uid="{B71808F8-FCFB-42D3-BF52-58D9E0580C1A}"/>
     <hyperlink ref="D14" r:id="rId10" display="https://www.amazon.com/gp/product/B083SGJ7BD/ref=ppx_yo_dt_b_search_asin_title?ie=UTF8&amp;psc=1" xr:uid="{DA66DF38-A09F-4211-8141-1818E8E255C7}"/>
-    <hyperlink ref="D15" r:id="rId11" display="https://www.amazon.com/gp/product/B06XP16Q4W/ref=ppx_yo_dt_b_asin_title_o01_s00?ie=UTF8&amp;th=1" xr:uid="{FF29243F-9608-467D-869E-7514D665C27E}"/>
-    <hyperlink ref="D16" r:id="rId12" display="https://www.amazon.com/gp/product/B08F77YVYB/ref=ppx_yo_dt_b_asin_title_o00_s00?ie=UTF8&amp;psc=1" xr:uid="{0751953C-478C-4815-94D1-AC08779238DF}"/>
-    <hyperlink ref="D17" r:id="rId13" display="https://www.amazon.com/Micro-Center-Class-Memory-Adapter/dp/B07K835MNR/ref=sr_1_36?dchild=1&amp;keywords=16gb+sd+card&amp;qid=1612732635&amp;sr=8-36" xr:uid="{0ED02E94-4D76-4658-8DE0-18A017F4CBA8}"/>
-    <hyperlink ref="D18" r:id="rId14" display="https://www.amazon.com/JXMOX-Charger-Charging-Compatible-2018-Grey/dp/B07TVMBZ75/ref=sr_1_3?dchild=1&amp;keywords=usb+c+to+usb+c+cable+short&amp;qid=1612732867&amp;sr=8-3" xr:uid="{A65511AB-084D-482E-ACC8-8AC38907AF9B}"/>
-    <hyperlink ref="D11" r:id="rId15" display="https://www.sparkfun.com/products/15448" xr:uid="{9716C4E0-BADF-4347-8019-72F83F0A0FEC}"/>
-    <hyperlink ref="D13" r:id="rId16" display="https://www.adafruit.com/product/2167" xr:uid="{F390DA11-248B-4D88-B312-4E370CAC65D6}"/>
+    <hyperlink ref="D15" r:id="rId11" display="https://www.amazon.com/gp/product/B08F77YVYB/ref=ppx_yo_dt_b_asin_title_o00_s00?ie=UTF8&amp;psc=1" xr:uid="{0751953C-478C-4815-94D1-AC08779238DF}"/>
+    <hyperlink ref="D16" r:id="rId12" display="https://www.amazon.com/Micro-Center-Class-Memory-Adapter/dp/B07K835MNR/ref=sr_1_36?dchild=1&amp;keywords=16gb+sd+card&amp;qid=1612732635&amp;sr=8-36" xr:uid="{0ED02E94-4D76-4658-8DE0-18A017F4CBA8}"/>
+    <hyperlink ref="D17" r:id="rId13" display="https://www.amazon.com/JXMOX-Charger-Charging-Compatible-2018-Grey/dp/B07TVMBZ75/ref=sr_1_3?dchild=1&amp;keywords=usb+c+to+usb+c+cable+short&amp;qid=1612732867&amp;sr=8-3" xr:uid="{A65511AB-084D-482E-ACC8-8AC38907AF9B}"/>
+    <hyperlink ref="D11" r:id="rId14" display="https://www.sparkfun.com/products/15448" xr:uid="{9716C4E0-BADF-4347-8019-72F83F0A0FEC}"/>
+    <hyperlink ref="D13" r:id="rId15" display="https://www.adafruit.com/product/2167" xr:uid="{F390DA11-248B-4D88-B312-4E370CAC65D6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId16"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated bom and resliced the cover and rpi mount
</commit_message>
<xml_diff>
--- a/hardware/dispenser/bom/precise_dispenser_bom.xlsx
+++ b/hardware/dispenser/bom/precise_dispenser_bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub Repos\canine_precise_dispenser\hardware\dispenser\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{373E15EE-16D5-4A6C-B7C2-ABB759896886}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7E0DCCD-7DCE-4CDA-BEEA-FBA1E735ABCA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -498,7 +498,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -537,10 +537,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="3">
-        <v>22.99</v>
+        <v>19.989999999999998</v>
       </c>
       <c r="D3" s="8" t="str">
-        <f>HYPERLINK("https://www.amazon.com/OVERTURE-Filament-Consumables-Dimensional-Accuracy/dp/B07PGY2JP1/ref=sr_1_9?crid=SP2VJ9AX94HN&amp;dchild=1&amp;keywords=1kg+pla+filament+1.75mm&amp;qid=1612737824&amp;sprefix=1kg+pla+%2Caps%2C223&amp;sr=8-9","Filament")</f>
+        <f>HYPERLINK("https://www.amazon.com/Inland-1-75mm-Natural-Printer-Filament/dp/B00YSP5SR8/ref=sr_1_3?dchild=1&amp;keywords=pla+filament+natural&amp;qid=1618415287&amp;sr=8-3","Filament")</f>
         <v>Filament</v>
       </c>
     </row>

</xml_diff>